<commit_message>
Changes made in Credit Report process
</commit_message>
<xml_diff>
--- a/Data/Input/CustomerCode/367/367.xlsx
+++ b/Data/Input/CustomerCode/367/367.xlsx
@@ -357,702 +357,702 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>700251</v>
+        <v>708029</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>700252</v>
+        <v>709970</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>700285</v>
+        <v>710180</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>701509</v>
+        <v>710515</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>701511</v>
+        <v>711279</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>702692</v>
+        <v>711347</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>703461</v>
+        <v>712758</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>704663</v>
+        <v>712779</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>704726</v>
+        <v>712785</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>706693</v>
+        <v>712806</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>706695</v>
+        <v>712807</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>706719</v>
+        <v>712980</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>707651</v>
+        <v>712981</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>708027</v>
+        <v>713946</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>807682</v>
+        <v>713947</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>807686</v>
+        <v>714821</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>807702</v>
+        <v>715549</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>807836</v>
+        <v>716045</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>808119</v>
+        <v>716223</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>808417</v>
+        <v>716786</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>808418</v>
+        <v>716961</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>808563</v>
+        <v>716965</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>808720</v>
+        <v>716973</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>808726</v>
+        <v>716986</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>808732</v>
+        <v>717051</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>808744</v>
+        <v>717175</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>809237</v>
+        <v>717220</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>809474</v>
+        <v>717850</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>708029</v>
+        <v>717901</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>709970</v>
+        <v>718092</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>710180</v>
+        <v>718093</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>710515</v>
+        <v>718095</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>711279</v>
+        <v>719381</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>711347</v>
+        <v>719387</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>712758</v>
+        <v>719444</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>712779</v>
+        <v>719506</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>712785</v>
+        <v>720032</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>712806</v>
+        <v>720121</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>712807</v>
+        <v>720146</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>712980</v>
+        <v>720188</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>712981</v>
+        <v>720475</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>713946</v>
+        <v>720479</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>713947</v>
+        <v>720563</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>714821</v>
+        <v>720565</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>715549</v>
+        <v>720627</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>716045</v>
+        <v>720628</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>716223</v>
+        <v>720969</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>716786</v>
+        <v>720996</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>716961</v>
+        <v>721002</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>716965</v>
+        <v>721036</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>716973</v>
+        <v>721173</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>716986</v>
+        <v>721363</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>717051</v>
+        <v>721370</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>717175</v>
+        <v>721374</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>717220</v>
+        <v>721380</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>717850</v>
+        <v>721391</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>717901</v>
+        <v>721393</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>718092</v>
+        <v>721423</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>718093</v>
+        <v>721430</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>718095</v>
+        <v>721456</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>719381</v>
+        <v>721476</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>719387</v>
+        <v>721578</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>719444</v>
+        <v>721676</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>719506</v>
+        <v>721767</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>720032</v>
+        <v>721773</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>720121</v>
+        <v>722001</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>720146</v>
+        <v>722003</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>720188</v>
+        <v>722088</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>720475</v>
+        <v>722116</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>720479</v>
+        <v>722120</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>720563</v>
+        <v>722121</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>720565</v>
+        <v>722164</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>720627</v>
+        <v>722298</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>720628</v>
+        <v>722299</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>720969</v>
+        <v>722307</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>720996</v>
+        <v>722310</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>721002</v>
+        <v>722344</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>721036</v>
+        <v>722345</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>721173</v>
+        <v>722351</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>721363</v>
+        <v>722352</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>721370</v>
+        <v>722371</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>721374</v>
+        <v>722374</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>721380</v>
+        <v>722375</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>721391</v>
+        <v>722403</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>721393</v>
+        <v>722449</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>721423</v>
+        <v>722451</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>721430</v>
+        <v>722453</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>721456</v>
+        <v>722454</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>721476</v>
+        <v>722455</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>721578</v>
+        <v>722667</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>721676</v>
+        <v>722772</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>721767</v>
+        <v>722773</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>721773</v>
+        <v>724033</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>722001</v>
+        <v>724098</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>722003</v>
+        <v>724413</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>722088</v>
+        <v>724459</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>722116</v>
+        <v>724460</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>722120</v>
+        <v>724527</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>722121</v>
+        <v>724642</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>722164</v>
+        <v>724655</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>722298</v>
+        <v>724752</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>722299</v>
+        <v>724765</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>722307</v>
+        <v>724767</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>722310</v>
+        <v>724773</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>722344</v>
+        <v>800029</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>722345</v>
+        <v>803783</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>722351</v>
+        <v>805844</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>722352</v>
+        <v>807670</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>722371</v>
+        <v>807672</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>722374</v>
+        <v>807674</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>722375</v>
+        <v>807676</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>722403</v>
+        <v>807678</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>722449</v>
+        <v>700251</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>722451</v>
+        <v>700252</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>722453</v>
+        <v>700285</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>722454</v>
+        <v>701509</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>722455</v>
+        <v>701511</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>722667</v>
+        <v>702692</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>722772</v>
+        <v>703461</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>722773</v>
+        <v>704663</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>724033</v>
+        <v>704726</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>724098</v>
+        <v>706693</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>724413</v>
+        <v>706695</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>724459</v>
+        <v>706719</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>724460</v>
+        <v>707651</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>724527</v>
+        <v>708027</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>724642</v>
+        <v>807682</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>724655</v>
+        <v>807686</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>724752</v>
+        <v>807702</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>724765</v>
+        <v>807836</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>724767</v>
+        <v>808119</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>724773</v>
+        <v>808417</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>800029</v>
+        <v>808418</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>803783</v>
+        <v>808563</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>805844</v>
+        <v>808720</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>807670</v>
+        <v>808726</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>807672</v>
+        <v>808732</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>807674</v>
+        <v>808744</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>807676</v>
+        <v>809237</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>807678</v>
+        <v>809474</v>
       </c>
     </row>
   </sheetData>

</xml_diff>